<commit_message>
style some gui real quick
</commit_message>
<xml_diff>
--- a/TC Form Generator/studentList.xlsx
+++ b/TC Form Generator/studentList.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995CBF50-F47B-4062-9BD7-8347335ED059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578E0327-33CF-4138-BBAC-488B4F765844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="244">
   <si>
     <t>sub1</t>
   </si>
@@ -735,6 +735,24 @@
   </si>
   <si>
     <t>SMQ 232/4 Air Force Station Darjipura Vadodara</t>
+  </si>
+  <si>
+    <t>phy</t>
+  </si>
+  <si>
+    <t>chem</t>
+  </si>
+  <si>
+    <t>maths</t>
+  </si>
+  <si>
+    <t>cs</t>
+  </si>
+  <si>
+    <t>hindi</t>
+  </si>
+  <si>
+    <t>bio</t>
   </si>
 </sst>
 </file>
@@ -859,7 +877,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -874,11 +892,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1221,8 +1237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:O79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,8 +1247,7 @@
     <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29.28515625" customWidth="1"/>
     <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="8" customWidth="1"/>
-    <col min="6" max="7" width="11" customWidth="1"/>
+    <col min="5" max="7" width="11" customWidth="1"/>
     <col min="8" max="8" width="65.28515625" customWidth="1"/>
     <col min="9" max="9" width="17.28515625" customWidth="1"/>
     <col min="10" max="15" width="12" customWidth="1"/>
@@ -1251,7 +1266,7 @@
       <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1313,6 +1328,24 @@
       <c r="I2">
         <v>24102022</v>
       </c>
+      <c r="J2" t="s">
+        <v>238</v>
+      </c>
+      <c r="K2" t="s">
+        <v>239</v>
+      </c>
+      <c r="L2" t="s">
+        <v>240</v>
+      </c>
+      <c r="M2" t="s">
+        <v>241</v>
+      </c>
+      <c r="N2" t="s">
+        <v>242</v>
+      </c>
+      <c r="O2" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="3" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -1342,6 +1375,24 @@
       <c r="I3">
         <v>25102022</v>
       </c>
+      <c r="J3" t="s">
+        <v>238</v>
+      </c>
+      <c r="K3" t="s">
+        <v>239</v>
+      </c>
+      <c r="L3" t="s">
+        <v>240</v>
+      </c>
+      <c r="M3" t="s">
+        <v>241</v>
+      </c>
+      <c r="N3" t="s">
+        <v>242</v>
+      </c>
+      <c r="O3" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="4" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -1368,6 +1419,24 @@
       <c r="H4" s="3" t="s">
         <v>186</v>
       </c>
+      <c r="J4" t="s">
+        <v>238</v>
+      </c>
+      <c r="K4" t="s">
+        <v>239</v>
+      </c>
+      <c r="L4" t="s">
+        <v>240</v>
+      </c>
+      <c r="M4" t="s">
+        <v>241</v>
+      </c>
+      <c r="N4" t="s">
+        <v>242</v>
+      </c>
+      <c r="O4" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="5" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -1394,6 +1463,24 @@
       <c r="H5" s="3" t="s">
         <v>187</v>
       </c>
+      <c r="J5" t="s">
+        <v>238</v>
+      </c>
+      <c r="K5" t="s">
+        <v>239</v>
+      </c>
+      <c r="L5" t="s">
+        <v>240</v>
+      </c>
+      <c r="M5" t="s">
+        <v>241</v>
+      </c>
+      <c r="N5" t="s">
+        <v>242</v>
+      </c>
+      <c r="O5" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="6" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -1420,6 +1507,24 @@
       <c r="H6" s="3" t="s">
         <v>188</v>
       </c>
+      <c r="J6" t="s">
+        <v>238</v>
+      </c>
+      <c r="K6" t="s">
+        <v>239</v>
+      </c>
+      <c r="L6" t="s">
+        <v>240</v>
+      </c>
+      <c r="M6" t="s">
+        <v>241</v>
+      </c>
+      <c r="N6" t="s">
+        <v>242</v>
+      </c>
+      <c r="O6" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="7" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -1446,6 +1551,24 @@
       <c r="H7" s="3" t="s">
         <v>189</v>
       </c>
+      <c r="J7" t="s">
+        <v>238</v>
+      </c>
+      <c r="K7" t="s">
+        <v>239</v>
+      </c>
+      <c r="L7" t="s">
+        <v>240</v>
+      </c>
+      <c r="M7" t="s">
+        <v>241</v>
+      </c>
+      <c r="N7" t="s">
+        <v>242</v>
+      </c>
+      <c r="O7" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="8" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -1472,6 +1595,24 @@
       <c r="H8" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="J8" t="s">
+        <v>238</v>
+      </c>
+      <c r="K8" t="s">
+        <v>239</v>
+      </c>
+      <c r="L8" t="s">
+        <v>240</v>
+      </c>
+      <c r="M8" t="s">
+        <v>241</v>
+      </c>
+      <c r="N8" t="s">
+        <v>242</v>
+      </c>
+      <c r="O8" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -1498,6 +1639,24 @@
       <c r="H9" s="3" t="s">
         <v>191</v>
       </c>
+      <c r="J9" t="s">
+        <v>238</v>
+      </c>
+      <c r="K9" t="s">
+        <v>239</v>
+      </c>
+      <c r="L9" t="s">
+        <v>240</v>
+      </c>
+      <c r="M9" t="s">
+        <v>241</v>
+      </c>
+      <c r="N9" t="s">
+        <v>242</v>
+      </c>
+      <c r="O9" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="10" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -1524,6 +1683,24 @@
       <c r="H10" s="3" t="s">
         <v>192</v>
       </c>
+      <c r="J10" t="s">
+        <v>238</v>
+      </c>
+      <c r="K10" t="s">
+        <v>239</v>
+      </c>
+      <c r="L10" t="s">
+        <v>240</v>
+      </c>
+      <c r="M10" t="s">
+        <v>241</v>
+      </c>
+      <c r="N10" t="s">
+        <v>242</v>
+      </c>
+      <c r="O10" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="11" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11">
@@ -1550,6 +1727,24 @@
       <c r="H11" s="3" t="s">
         <v>193</v>
       </c>
+      <c r="J11" t="s">
+        <v>238</v>
+      </c>
+      <c r="K11" t="s">
+        <v>239</v>
+      </c>
+      <c r="L11" t="s">
+        <v>240</v>
+      </c>
+      <c r="M11" t="s">
+        <v>241</v>
+      </c>
+      <c r="N11" t="s">
+        <v>242</v>
+      </c>
+      <c r="O11" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12">
@@ -1576,6 +1771,24 @@
       <c r="H12" s="3" t="s">
         <v>194</v>
       </c>
+      <c r="J12" t="s">
+        <v>238</v>
+      </c>
+      <c r="K12" t="s">
+        <v>239</v>
+      </c>
+      <c r="L12" t="s">
+        <v>240</v>
+      </c>
+      <c r="M12" t="s">
+        <v>241</v>
+      </c>
+      <c r="N12" t="s">
+        <v>242</v>
+      </c>
+      <c r="O12" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -1602,6 +1815,24 @@
       <c r="H13" s="3" t="s">
         <v>195</v>
       </c>
+      <c r="J13" t="s">
+        <v>238</v>
+      </c>
+      <c r="K13" t="s">
+        <v>239</v>
+      </c>
+      <c r="L13" t="s">
+        <v>240</v>
+      </c>
+      <c r="M13" t="s">
+        <v>241</v>
+      </c>
+      <c r="N13" t="s">
+        <v>242</v>
+      </c>
+      <c r="O13" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -1628,6 +1859,24 @@
       <c r="H14" s="3" t="s">
         <v>196</v>
       </c>
+      <c r="J14" t="s">
+        <v>238</v>
+      </c>
+      <c r="K14" t="s">
+        <v>239</v>
+      </c>
+      <c r="L14" t="s">
+        <v>240</v>
+      </c>
+      <c r="M14" t="s">
+        <v>241</v>
+      </c>
+      <c r="N14" t="s">
+        <v>242</v>
+      </c>
+      <c r="O14" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="15" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -1654,6 +1903,24 @@
       <c r="H15" s="3" t="s">
         <v>197</v>
       </c>
+      <c r="J15" t="s">
+        <v>238</v>
+      </c>
+      <c r="K15" t="s">
+        <v>239</v>
+      </c>
+      <c r="L15" t="s">
+        <v>240</v>
+      </c>
+      <c r="M15" t="s">
+        <v>241</v>
+      </c>
+      <c r="N15" t="s">
+        <v>242</v>
+      </c>
+      <c r="O15" t="s">
+        <v>243</v>
+      </c>
     </row>
     <row r="16" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -1680,8 +1947,26 @@
       <c r="H16" s="3" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J16" t="s">
+        <v>238</v>
+      </c>
+      <c r="K16" t="s">
+        <v>239</v>
+      </c>
+      <c r="L16" t="s">
+        <v>240</v>
+      </c>
+      <c r="M16" t="s">
+        <v>241</v>
+      </c>
+      <c r="N16" t="s">
+        <v>242</v>
+      </c>
+      <c r="O16" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1249</v>
       </c>
@@ -1706,8 +1991,26 @@
       <c r="H17" s="3" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J17" t="s">
+        <v>238</v>
+      </c>
+      <c r="K17" t="s">
+        <v>239</v>
+      </c>
+      <c r="L17" t="s">
+        <v>240</v>
+      </c>
+      <c r="M17" t="s">
+        <v>241</v>
+      </c>
+      <c r="N17" t="s">
+        <v>242</v>
+      </c>
+      <c r="O17" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>1250</v>
       </c>
@@ -1732,8 +2035,26 @@
       <c r="H18" s="3" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J18" t="s">
+        <v>238</v>
+      </c>
+      <c r="K18" t="s">
+        <v>239</v>
+      </c>
+      <c r="L18" t="s">
+        <v>240</v>
+      </c>
+      <c r="M18" t="s">
+        <v>241</v>
+      </c>
+      <c r="N18" t="s">
+        <v>242</v>
+      </c>
+      <c r="O18" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1251</v>
       </c>
@@ -1758,8 +2079,26 @@
       <c r="H19" s="3" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J19" t="s">
+        <v>238</v>
+      </c>
+      <c r="K19" t="s">
+        <v>239</v>
+      </c>
+      <c r="L19" t="s">
+        <v>240</v>
+      </c>
+      <c r="M19" t="s">
+        <v>241</v>
+      </c>
+      <c r="N19" t="s">
+        <v>242</v>
+      </c>
+      <c r="O19" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1252</v>
       </c>
@@ -1784,8 +2123,26 @@
       <c r="H20" s="3" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J20" t="s">
+        <v>238</v>
+      </c>
+      <c r="K20" t="s">
+        <v>239</v>
+      </c>
+      <c r="L20" t="s">
+        <v>240</v>
+      </c>
+      <c r="M20" t="s">
+        <v>241</v>
+      </c>
+      <c r="N20" t="s">
+        <v>242</v>
+      </c>
+      <c r="O20" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1253</v>
       </c>
@@ -1810,8 +2167,26 @@
       <c r="H21" s="3" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J21" t="s">
+        <v>238</v>
+      </c>
+      <c r="K21" t="s">
+        <v>239</v>
+      </c>
+      <c r="L21" t="s">
+        <v>240</v>
+      </c>
+      <c r="M21" t="s">
+        <v>241</v>
+      </c>
+      <c r="N21" t="s">
+        <v>242</v>
+      </c>
+      <c r="O21" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>1254</v>
       </c>
@@ -1836,8 +2211,26 @@
       <c r="H22" s="3" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J22" t="s">
+        <v>238</v>
+      </c>
+      <c r="K22" t="s">
+        <v>239</v>
+      </c>
+      <c r="L22" t="s">
+        <v>240</v>
+      </c>
+      <c r="M22" t="s">
+        <v>241</v>
+      </c>
+      <c r="N22" t="s">
+        <v>242</v>
+      </c>
+      <c r="O22" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>1255</v>
       </c>
@@ -1862,8 +2255,26 @@
       <c r="H23" s="3" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J23" t="s">
+        <v>238</v>
+      </c>
+      <c r="K23" t="s">
+        <v>239</v>
+      </c>
+      <c r="L23" t="s">
+        <v>240</v>
+      </c>
+      <c r="M23" t="s">
+        <v>241</v>
+      </c>
+      <c r="N23" t="s">
+        <v>242</v>
+      </c>
+      <c r="O23" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1256</v>
       </c>
@@ -1888,8 +2299,26 @@
       <c r="H24" s="3" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J24" t="s">
+        <v>238</v>
+      </c>
+      <c r="K24" t="s">
+        <v>239</v>
+      </c>
+      <c r="L24" t="s">
+        <v>240</v>
+      </c>
+      <c r="M24" t="s">
+        <v>241</v>
+      </c>
+      <c r="N24" t="s">
+        <v>242</v>
+      </c>
+      <c r="O24" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>1257</v>
       </c>
@@ -1914,8 +2343,26 @@
       <c r="H25" s="3" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J25" t="s">
+        <v>238</v>
+      </c>
+      <c r="K25" t="s">
+        <v>239</v>
+      </c>
+      <c r="L25" t="s">
+        <v>240</v>
+      </c>
+      <c r="M25" t="s">
+        <v>241</v>
+      </c>
+      <c r="N25" t="s">
+        <v>242</v>
+      </c>
+      <c r="O25" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1258</v>
       </c>
@@ -1940,8 +2387,26 @@
       <c r="H26" s="3" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J26" t="s">
+        <v>238</v>
+      </c>
+      <c r="K26" t="s">
+        <v>239</v>
+      </c>
+      <c r="L26" t="s">
+        <v>240</v>
+      </c>
+      <c r="M26" t="s">
+        <v>241</v>
+      </c>
+      <c r="N26" t="s">
+        <v>242</v>
+      </c>
+      <c r="O26" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>1259</v>
       </c>
@@ -1966,8 +2431,26 @@
       <c r="H27" s="3" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J27" t="s">
+        <v>238</v>
+      </c>
+      <c r="K27" t="s">
+        <v>239</v>
+      </c>
+      <c r="L27" t="s">
+        <v>240</v>
+      </c>
+      <c r="M27" t="s">
+        <v>241</v>
+      </c>
+      <c r="N27" t="s">
+        <v>242</v>
+      </c>
+      <c r="O27" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1260</v>
       </c>
@@ -1992,8 +2475,26 @@
       <c r="H28" s="3" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J28" t="s">
+        <v>238</v>
+      </c>
+      <c r="K28" t="s">
+        <v>239</v>
+      </c>
+      <c r="L28" t="s">
+        <v>240</v>
+      </c>
+      <c r="M28" t="s">
+        <v>241</v>
+      </c>
+      <c r="N28" t="s">
+        <v>242</v>
+      </c>
+      <c r="O28" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>1261</v>
       </c>
@@ -2018,8 +2519,26 @@
       <c r="H29" s="3" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J29" t="s">
+        <v>238</v>
+      </c>
+      <c r="K29" t="s">
+        <v>239</v>
+      </c>
+      <c r="L29" t="s">
+        <v>240</v>
+      </c>
+      <c r="M29" t="s">
+        <v>241</v>
+      </c>
+      <c r="N29" t="s">
+        <v>242</v>
+      </c>
+      <c r="O29" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>1262</v>
       </c>
@@ -2044,8 +2563,26 @@
       <c r="H30" s="3" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J30" t="s">
+        <v>238</v>
+      </c>
+      <c r="K30" t="s">
+        <v>239</v>
+      </c>
+      <c r="L30" t="s">
+        <v>240</v>
+      </c>
+      <c r="M30" t="s">
+        <v>241</v>
+      </c>
+      <c r="N30" t="s">
+        <v>242</v>
+      </c>
+      <c r="O30" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>1263</v>
       </c>
@@ -2070,8 +2607,26 @@
       <c r="H31" s="3" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J31" t="s">
+        <v>238</v>
+      </c>
+      <c r="K31" t="s">
+        <v>239</v>
+      </c>
+      <c r="L31" t="s">
+        <v>240</v>
+      </c>
+      <c r="M31" t="s">
+        <v>241</v>
+      </c>
+      <c r="N31" t="s">
+        <v>242</v>
+      </c>
+      <c r="O31" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1264</v>
       </c>
@@ -2096,8 +2651,26 @@
       <c r="H32" s="3" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J32" t="s">
+        <v>238</v>
+      </c>
+      <c r="K32" t="s">
+        <v>239</v>
+      </c>
+      <c r="L32" t="s">
+        <v>240</v>
+      </c>
+      <c r="M32" t="s">
+        <v>241</v>
+      </c>
+      <c r="N32" t="s">
+        <v>242</v>
+      </c>
+      <c r="O32" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1265</v>
       </c>
@@ -2122,8 +2695,26 @@
       <c r="H33" s="3" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J33" t="s">
+        <v>238</v>
+      </c>
+      <c r="K33" t="s">
+        <v>239</v>
+      </c>
+      <c r="L33" t="s">
+        <v>240</v>
+      </c>
+      <c r="M33" t="s">
+        <v>241</v>
+      </c>
+      <c r="N33" t="s">
+        <v>242</v>
+      </c>
+      <c r="O33" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>1266</v>
       </c>
@@ -2148,8 +2739,26 @@
       <c r="H34" s="3" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J34" t="s">
+        <v>238</v>
+      </c>
+      <c r="K34" t="s">
+        <v>239</v>
+      </c>
+      <c r="L34" t="s">
+        <v>240</v>
+      </c>
+      <c r="M34" t="s">
+        <v>241</v>
+      </c>
+      <c r="N34" t="s">
+        <v>242</v>
+      </c>
+      <c r="O34" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>1267</v>
       </c>
@@ -2174,8 +2783,26 @@
       <c r="H35" s="3" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J35" t="s">
+        <v>238</v>
+      </c>
+      <c r="K35" t="s">
+        <v>239</v>
+      </c>
+      <c r="L35" t="s">
+        <v>240</v>
+      </c>
+      <c r="M35" t="s">
+        <v>241</v>
+      </c>
+      <c r="N35" t="s">
+        <v>242</v>
+      </c>
+      <c r="O35" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1268</v>
       </c>
@@ -2200,8 +2827,26 @@
       <c r="H36" s="3" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J36" t="s">
+        <v>238</v>
+      </c>
+      <c r="K36" t="s">
+        <v>239</v>
+      </c>
+      <c r="L36" t="s">
+        <v>240</v>
+      </c>
+      <c r="M36" t="s">
+        <v>241</v>
+      </c>
+      <c r="N36" t="s">
+        <v>242</v>
+      </c>
+      <c r="O36" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>1269</v>
       </c>
@@ -2226,8 +2871,26 @@
       <c r="H37" s="3" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J37" t="s">
+        <v>238</v>
+      </c>
+      <c r="K37" t="s">
+        <v>239</v>
+      </c>
+      <c r="L37" t="s">
+        <v>240</v>
+      </c>
+      <c r="M37" t="s">
+        <v>241</v>
+      </c>
+      <c r="N37" t="s">
+        <v>242</v>
+      </c>
+      <c r="O37" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1270</v>
       </c>
@@ -2252,8 +2915,26 @@
       <c r="H38" s="3" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J38" t="s">
+        <v>238</v>
+      </c>
+      <c r="K38" t="s">
+        <v>239</v>
+      </c>
+      <c r="L38" t="s">
+        <v>240</v>
+      </c>
+      <c r="M38" t="s">
+        <v>241</v>
+      </c>
+      <c r="N38" t="s">
+        <v>242</v>
+      </c>
+      <c r="O38" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>1271</v>
       </c>
@@ -2278,8 +2959,26 @@
       <c r="H39" s="3" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J39" t="s">
+        <v>238</v>
+      </c>
+      <c r="K39" t="s">
+        <v>239</v>
+      </c>
+      <c r="L39" t="s">
+        <v>240</v>
+      </c>
+      <c r="M39" t="s">
+        <v>241</v>
+      </c>
+      <c r="N39" t="s">
+        <v>242</v>
+      </c>
+      <c r="O39" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1272</v>
       </c>
@@ -2304,8 +3003,26 @@
       <c r="H40" s="3" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J40" t="s">
+        <v>238</v>
+      </c>
+      <c r="K40" t="s">
+        <v>239</v>
+      </c>
+      <c r="L40" t="s">
+        <v>240</v>
+      </c>
+      <c r="M40" t="s">
+        <v>241</v>
+      </c>
+      <c r="N40" t="s">
+        <v>242</v>
+      </c>
+      <c r="O40" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>1273</v>
       </c>
@@ -2330,8 +3047,26 @@
       <c r="H41" s="3" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J41" t="s">
+        <v>238</v>
+      </c>
+      <c r="K41" t="s">
+        <v>239</v>
+      </c>
+      <c r="L41" t="s">
+        <v>240</v>
+      </c>
+      <c r="M41" t="s">
+        <v>241</v>
+      </c>
+      <c r="N41" t="s">
+        <v>242</v>
+      </c>
+      <c r="O41" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1274</v>
       </c>
@@ -2356,8 +3091,26 @@
       <c r="H42" s="3" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J42" t="s">
+        <v>238</v>
+      </c>
+      <c r="K42" t="s">
+        <v>239</v>
+      </c>
+      <c r="L42" t="s">
+        <v>240</v>
+      </c>
+      <c r="M42" t="s">
+        <v>241</v>
+      </c>
+      <c r="N42" t="s">
+        <v>242</v>
+      </c>
+      <c r="O42" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>1275</v>
       </c>
@@ -2382,8 +3135,26 @@
       <c r="H43" s="3" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J43" t="s">
+        <v>238</v>
+      </c>
+      <c r="K43" t="s">
+        <v>239</v>
+      </c>
+      <c r="L43" t="s">
+        <v>240</v>
+      </c>
+      <c r="M43" t="s">
+        <v>241</v>
+      </c>
+      <c r="N43" t="s">
+        <v>242</v>
+      </c>
+      <c r="O43" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>1276</v>
       </c>
@@ -2408,8 +3179,26 @@
       <c r="H44" s="3" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J44" t="s">
+        <v>238</v>
+      </c>
+      <c r="K44" t="s">
+        <v>239</v>
+      </c>
+      <c r="L44" t="s">
+        <v>240</v>
+      </c>
+      <c r="M44" t="s">
+        <v>241</v>
+      </c>
+      <c r="N44" t="s">
+        <v>242</v>
+      </c>
+      <c r="O44" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>1277</v>
       </c>
@@ -2434,8 +3223,26 @@
       <c r="H45" s="3" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J45" t="s">
+        <v>238</v>
+      </c>
+      <c r="K45" t="s">
+        <v>239</v>
+      </c>
+      <c r="L45" t="s">
+        <v>240</v>
+      </c>
+      <c r="M45" t="s">
+        <v>241</v>
+      </c>
+      <c r="N45" t="s">
+        <v>242</v>
+      </c>
+      <c r="O45" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>1278</v>
       </c>
@@ -2460,8 +3267,26 @@
       <c r="H46" s="3" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J46" t="s">
+        <v>238</v>
+      </c>
+      <c r="K46" t="s">
+        <v>239</v>
+      </c>
+      <c r="L46" t="s">
+        <v>240</v>
+      </c>
+      <c r="M46" t="s">
+        <v>241</v>
+      </c>
+      <c r="N46" t="s">
+        <v>242</v>
+      </c>
+      <c r="O46" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>1279</v>
       </c>
@@ -2486,8 +3311,26 @@
       <c r="H47" s="3" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J47" t="s">
+        <v>238</v>
+      </c>
+      <c r="K47" t="s">
+        <v>239</v>
+      </c>
+      <c r="L47" t="s">
+        <v>240</v>
+      </c>
+      <c r="M47" t="s">
+        <v>241</v>
+      </c>
+      <c r="N47" t="s">
+        <v>242</v>
+      </c>
+      <c r="O47" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>1280</v>
       </c>
@@ -2512,8 +3355,26 @@
       <c r="H48" s="3" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J48" t="s">
+        <v>238</v>
+      </c>
+      <c r="K48" t="s">
+        <v>239</v>
+      </c>
+      <c r="L48" t="s">
+        <v>240</v>
+      </c>
+      <c r="M48" t="s">
+        <v>241</v>
+      </c>
+      <c r="N48" t="s">
+        <v>242</v>
+      </c>
+      <c r="O48" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>1281</v>
       </c>
@@ -2538,8 +3399,26 @@
       <c r="H49" s="3" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J49" t="s">
+        <v>238</v>
+      </c>
+      <c r="K49" t="s">
+        <v>239</v>
+      </c>
+      <c r="L49" t="s">
+        <v>240</v>
+      </c>
+      <c r="M49" t="s">
+        <v>241</v>
+      </c>
+      <c r="N49" t="s">
+        <v>242</v>
+      </c>
+      <c r="O49" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1282</v>
       </c>
@@ -2564,8 +3443,26 @@
       <c r="H50" s="3" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J50" t="s">
+        <v>238</v>
+      </c>
+      <c r="K50" t="s">
+        <v>239</v>
+      </c>
+      <c r="L50" t="s">
+        <v>240</v>
+      </c>
+      <c r="M50" t="s">
+        <v>241</v>
+      </c>
+      <c r="N50" t="s">
+        <v>242</v>
+      </c>
+      <c r="O50" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>1283</v>
       </c>
@@ -2590,8 +3487,26 @@
       <c r="H51" s="3" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J51" t="s">
+        <v>238</v>
+      </c>
+      <c r="K51" t="s">
+        <v>239</v>
+      </c>
+      <c r="L51" t="s">
+        <v>240</v>
+      </c>
+      <c r="M51" t="s">
+        <v>241</v>
+      </c>
+      <c r="N51" t="s">
+        <v>242</v>
+      </c>
+      <c r="O51" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>1284</v>
       </c>
@@ -2616,8 +3531,26 @@
       <c r="H52" s="3" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J52" t="s">
+        <v>238</v>
+      </c>
+      <c r="K52" t="s">
+        <v>239</v>
+      </c>
+      <c r="L52" t="s">
+        <v>240</v>
+      </c>
+      <c r="M52" t="s">
+        <v>241</v>
+      </c>
+      <c r="N52" t="s">
+        <v>242</v>
+      </c>
+      <c r="O52" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>1285</v>
       </c>
@@ -2640,8 +3573,26 @@
         <v>7</v>
       </c>
       <c r="H53" s="4"/>
-    </row>
-    <row r="54" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J53" t="s">
+        <v>238</v>
+      </c>
+      <c r="K53" t="s">
+        <v>239</v>
+      </c>
+      <c r="L53" t="s">
+        <v>240</v>
+      </c>
+      <c r="M53" t="s">
+        <v>241</v>
+      </c>
+      <c r="N53" t="s">
+        <v>242</v>
+      </c>
+      <c r="O53" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1286</v>
       </c>
@@ -2666,8 +3617,26 @@
       <c r="H54" s="4" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J54" t="s">
+        <v>238</v>
+      </c>
+      <c r="K54" t="s">
+        <v>239</v>
+      </c>
+      <c r="L54" t="s">
+        <v>240</v>
+      </c>
+      <c r="M54" t="s">
+        <v>241</v>
+      </c>
+      <c r="N54" t="s">
+        <v>242</v>
+      </c>
+      <c r="O54" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>1287</v>
       </c>
@@ -2692,8 +3661,26 @@
       <c r="H55" s="4" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J55" t="s">
+        <v>238</v>
+      </c>
+      <c r="K55" t="s">
+        <v>239</v>
+      </c>
+      <c r="L55" t="s">
+        <v>240</v>
+      </c>
+      <c r="M55" t="s">
+        <v>241</v>
+      </c>
+      <c r="N55" t="s">
+        <v>242</v>
+      </c>
+      <c r="O55" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>1288</v>
       </c>
@@ -2718,8 +3705,26 @@
       <c r="H56" s="4" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J56" t="s">
+        <v>238</v>
+      </c>
+      <c r="K56" t="s">
+        <v>239</v>
+      </c>
+      <c r="L56" t="s">
+        <v>240</v>
+      </c>
+      <c r="M56" t="s">
+        <v>241</v>
+      </c>
+      <c r="N56" t="s">
+        <v>242</v>
+      </c>
+      <c r="O56" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>1289</v>
       </c>
@@ -2744,8 +3749,26 @@
       <c r="H57" s="4" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J57" t="s">
+        <v>238</v>
+      </c>
+      <c r="K57" t="s">
+        <v>239</v>
+      </c>
+      <c r="L57" t="s">
+        <v>240</v>
+      </c>
+      <c r="M57" t="s">
+        <v>241</v>
+      </c>
+      <c r="N57" t="s">
+        <v>242</v>
+      </c>
+      <c r="O57" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>1290</v>
       </c>
@@ -2764,8 +3787,26 @@
         <v>7</v>
       </c>
       <c r="H58" s="4"/>
-    </row>
-    <row r="59" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J58" t="s">
+        <v>238</v>
+      </c>
+      <c r="K58" t="s">
+        <v>239</v>
+      </c>
+      <c r="L58" t="s">
+        <v>240</v>
+      </c>
+      <c r="M58" t="s">
+        <v>241</v>
+      </c>
+      <c r="N58" t="s">
+        <v>242</v>
+      </c>
+      <c r="O58" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>1291</v>
       </c>
@@ -2790,126 +3831,504 @@
       <c r="H59" s="4" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J59" t="s">
+        <v>238</v>
+      </c>
+      <c r="K59" t="s">
+        <v>239</v>
+      </c>
+      <c r="L59" t="s">
+        <v>240</v>
+      </c>
+      <c r="M59" t="s">
+        <v>241</v>
+      </c>
+      <c r="N59" t="s">
+        <v>242</v>
+      </c>
+      <c r="O59" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1292</v>
       </c>
       <c r="E60" s="6"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J60" t="s">
+        <v>238</v>
+      </c>
+      <c r="K60" t="s">
+        <v>239</v>
+      </c>
+      <c r="L60" t="s">
+        <v>240</v>
+      </c>
+      <c r="M60" t="s">
+        <v>241</v>
+      </c>
+      <c r="N60" t="s">
+        <v>242</v>
+      </c>
+      <c r="O60" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1293</v>
       </c>
       <c r="E61" s="6"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J61" t="s">
+        <v>238</v>
+      </c>
+      <c r="K61" t="s">
+        <v>239</v>
+      </c>
+      <c r="L61" t="s">
+        <v>240</v>
+      </c>
+      <c r="M61" t="s">
+        <v>241</v>
+      </c>
+      <c r="N61" t="s">
+        <v>242</v>
+      </c>
+      <c r="O61" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1294</v>
       </c>
       <c r="E62" s="6"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J62" t="s">
+        <v>238</v>
+      </c>
+      <c r="K62" t="s">
+        <v>239</v>
+      </c>
+      <c r="L62" t="s">
+        <v>240</v>
+      </c>
+      <c r="M62" t="s">
+        <v>241</v>
+      </c>
+      <c r="N62" t="s">
+        <v>242</v>
+      </c>
+      <c r="O62" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1295</v>
       </c>
       <c r="E63" s="6"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J63" t="s">
+        <v>238</v>
+      </c>
+      <c r="K63" t="s">
+        <v>239</v>
+      </c>
+      <c r="L63" t="s">
+        <v>240</v>
+      </c>
+      <c r="M63" t="s">
+        <v>241</v>
+      </c>
+      <c r="N63" t="s">
+        <v>242</v>
+      </c>
+      <c r="O63" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1296</v>
       </c>
       <c r="E64" s="6"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J64" t="s">
+        <v>238</v>
+      </c>
+      <c r="K64" t="s">
+        <v>239</v>
+      </c>
+      <c r="L64" t="s">
+        <v>240</v>
+      </c>
+      <c r="M64" t="s">
+        <v>241</v>
+      </c>
+      <c r="N64" t="s">
+        <v>242</v>
+      </c>
+      <c r="O64" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1297</v>
       </c>
       <c r="E65" s="6"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J65" t="s">
+        <v>238</v>
+      </c>
+      <c r="K65" t="s">
+        <v>239</v>
+      </c>
+      <c r="L65" t="s">
+        <v>240</v>
+      </c>
+      <c r="M65" t="s">
+        <v>241</v>
+      </c>
+      <c r="N65" t="s">
+        <v>242</v>
+      </c>
+      <c r="O65" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1298</v>
       </c>
       <c r="E66" s="6"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J66" t="s">
+        <v>238</v>
+      </c>
+      <c r="K66" t="s">
+        <v>239</v>
+      </c>
+      <c r="L66" t="s">
+        <v>240</v>
+      </c>
+      <c r="M66" t="s">
+        <v>241</v>
+      </c>
+      <c r="N66" t="s">
+        <v>242</v>
+      </c>
+      <c r="O66" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1299</v>
       </c>
       <c r="E67" s="6"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J67" t="s">
+        <v>238</v>
+      </c>
+      <c r="K67" t="s">
+        <v>239</v>
+      </c>
+      <c r="L67" t="s">
+        <v>240</v>
+      </c>
+      <c r="M67" t="s">
+        <v>241</v>
+      </c>
+      <c r="N67" t="s">
+        <v>242</v>
+      </c>
+      <c r="O67" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1300</v>
       </c>
       <c r="E68" s="6"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J68" t="s">
+        <v>238</v>
+      </c>
+      <c r="K68" t="s">
+        <v>239</v>
+      </c>
+      <c r="L68" t="s">
+        <v>240</v>
+      </c>
+      <c r="M68" t="s">
+        <v>241</v>
+      </c>
+      <c r="N68" t="s">
+        <v>242</v>
+      </c>
+      <c r="O68" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1301</v>
       </c>
       <c r="E69" s="6"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J69" t="s">
+        <v>238</v>
+      </c>
+      <c r="K69" t="s">
+        <v>239</v>
+      </c>
+      <c r="L69" t="s">
+        <v>240</v>
+      </c>
+      <c r="M69" t="s">
+        <v>241</v>
+      </c>
+      <c r="N69" t="s">
+        <v>242</v>
+      </c>
+      <c r="O69" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1302</v>
       </c>
       <c r="E70" s="6"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J70" t="s">
+        <v>238</v>
+      </c>
+      <c r="K70" t="s">
+        <v>239</v>
+      </c>
+      <c r="L70" t="s">
+        <v>240</v>
+      </c>
+      <c r="M70" t="s">
+        <v>241</v>
+      </c>
+      <c r="N70" t="s">
+        <v>242</v>
+      </c>
+      <c r="O70" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1303</v>
       </c>
       <c r="E71" s="6"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J71" t="s">
+        <v>238</v>
+      </c>
+      <c r="K71" t="s">
+        <v>239</v>
+      </c>
+      <c r="L71" t="s">
+        <v>240</v>
+      </c>
+      <c r="M71" t="s">
+        <v>241</v>
+      </c>
+      <c r="N71" t="s">
+        <v>242</v>
+      </c>
+      <c r="O71" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1304</v>
       </c>
       <c r="E72" s="6"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J72" t="s">
+        <v>238</v>
+      </c>
+      <c r="K72" t="s">
+        <v>239</v>
+      </c>
+      <c r="L72" t="s">
+        <v>240</v>
+      </c>
+      <c r="M72" t="s">
+        <v>241</v>
+      </c>
+      <c r="N72" t="s">
+        <v>242</v>
+      </c>
+      <c r="O72" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1305</v>
       </c>
       <c r="E73" s="6"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J73" t="s">
+        <v>238</v>
+      </c>
+      <c r="K73" t="s">
+        <v>239</v>
+      </c>
+      <c r="L73" t="s">
+        <v>240</v>
+      </c>
+      <c r="M73" t="s">
+        <v>241</v>
+      </c>
+      <c r="N73" t="s">
+        <v>242</v>
+      </c>
+      <c r="O73" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1306</v>
       </c>
       <c r="E74" s="6"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J74" t="s">
+        <v>238</v>
+      </c>
+      <c r="K74" t="s">
+        <v>239</v>
+      </c>
+      <c r="L74" t="s">
+        <v>240</v>
+      </c>
+      <c r="M74" t="s">
+        <v>241</v>
+      </c>
+      <c r="N74" t="s">
+        <v>242</v>
+      </c>
+      <c r="O74" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1307</v>
       </c>
       <c r="E75" s="6"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J75" t="s">
+        <v>238</v>
+      </c>
+      <c r="K75" t="s">
+        <v>239</v>
+      </c>
+      <c r="L75" t="s">
+        <v>240</v>
+      </c>
+      <c r="M75" t="s">
+        <v>241</v>
+      </c>
+      <c r="N75" t="s">
+        <v>242</v>
+      </c>
+      <c r="O75" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>1308</v>
       </c>
       <c r="E76" s="6"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J76" t="s">
+        <v>238</v>
+      </c>
+      <c r="K76" t="s">
+        <v>239</v>
+      </c>
+      <c r="L76" t="s">
+        <v>240</v>
+      </c>
+      <c r="M76" t="s">
+        <v>241</v>
+      </c>
+      <c r="N76" t="s">
+        <v>242</v>
+      </c>
+      <c r="O76" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>1309</v>
       </c>
       <c r="E77" s="6"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J77" t="s">
+        <v>238</v>
+      </c>
+      <c r="K77" t="s">
+        <v>239</v>
+      </c>
+      <c r="L77" t="s">
+        <v>240</v>
+      </c>
+      <c r="M77" t="s">
+        <v>241</v>
+      </c>
+      <c r="N77" t="s">
+        <v>242</v>
+      </c>
+      <c r="O77" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1310</v>
       </c>
       <c r="E78" s="6"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J78" t="s">
+        <v>238</v>
+      </c>
+      <c r="K78" t="s">
+        <v>239</v>
+      </c>
+      <c r="L78" t="s">
+        <v>240</v>
+      </c>
+      <c r="M78" t="s">
+        <v>241</v>
+      </c>
+      <c r="N78" t="s">
+        <v>242</v>
+      </c>
+      <c r="O78" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1311</v>
       </c>
       <c r="E79" s="6"/>
+      <c r="J79" t="s">
+        <v>238</v>
+      </c>
+      <c r="K79" t="s">
+        <v>239</v>
+      </c>
+      <c r="L79" t="s">
+        <v>240</v>
+      </c>
+      <c r="M79" t="s">
+        <v>241</v>
+      </c>
+      <c r="N79" t="s">
+        <v>242</v>
+      </c>
+      <c r="O79" t="s">
+        <v>243</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>